<commit_message>
Update Excel Rows by PUT request
</commit_message>
<xml_diff>
--- a/public/temmuz 2024 dene.xlsx
+++ b/public/temmuz 2024 dene.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\-Downloads-\Study\BM\Staj\2 MaPos\Meyvalı Lokantası\meyvali-excel\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE02DC-ED96-4F19-A2EE-803763B58010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89B12A4-2198-4CA9-B0DF-9A83CE1638B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -394,6 +394,9 @@
     <t>Adisyon ve tahsilat yönetimi ; tahsilatlar veresiye hanesinden ( veya tahsil edilmiş adisyondan düşülecek )</t>
   </si>
   <si>
+    <t>Tarih</t>
+  </si>
+  <si>
     <t>Katagori</t>
   </si>
   <si>
@@ -412,22 +415,19 @@
     <t>Ek Bilgi</t>
   </si>
   <si>
+    <t>Bimden Et</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
     <t>Nakit</t>
   </si>
   <si>
-    <t>Bimden Et</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
     <t>5 Ekmek</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Tarih</t>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2812,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -2820,34 +2820,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="7" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2867,7 +2863,7 @@
         <v>127</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G2" t="s">
         <v>67</v>
@@ -2881,13 +2877,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F3" t="s">
         <v>66</v>
@@ -2896,12 +2892,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:G1 A2:G3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>